<commit_message>
p_dispatch and p_store read
Hydro still has some troubles in modelling
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\smspp-project\transformation_pypsa_smspp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\sms\transformation_pypsa_smspp\pypsa2smspp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -377,6 +377,12 @@
   </si>
   <si>
     <t>ActivePowerCost</t>
+  </si>
+  <si>
+    <t>[NR]</t>
+  </si>
+  <si>
+    <t>[NP] | [T][NP]</t>
   </si>
 </sst>
 </file>
@@ -702,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1600,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1948,7 +1954,7 @@
         <v>106</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>14</v>
@@ -2088,7 +2094,7 @@
         <v>106</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
First implementation idea of investmentblock
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
     <sheet name="ThermalUnitBlock" sheetId="2" r:id="rId2"/>
     <sheet name="BatteryUnitBlock" sheetId="3" r:id="rId3"/>
     <sheet name="HydroUnitBlock" sheetId="4" r:id="rId4"/>
-    <sheet name="Lines" sheetId="5" r:id="rId5"/>
-    <sheet name="Links" sheetId="6" r:id="rId6"/>
+    <sheet name="InvestmentBlock" sheetId="7" r:id="rId5"/>
+    <sheet name="Lines" sheetId="5" r:id="rId6"/>
+    <sheet name="Links" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="125">
   <si>
     <t>Name</t>
   </si>
@@ -383,6 +384,27 @@
   </si>
   <si>
     <t>[NP] | [T][NP]</t>
+  </si>
+  <si>
+    <t>Capital cost</t>
+  </si>
+  <si>
+    <t>LowerBound</t>
+  </si>
+  <si>
+    <t>Minimum acceptable size</t>
+  </si>
+  <si>
+    <t>UpperBound</t>
+  </si>
+  <si>
+    <t>Maximum acceptable size</t>
+  </si>
+  <si>
+    <t>InstalledCapacity</t>
+  </si>
+  <si>
+    <t>Installed capacity</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1280,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1606,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -2107,6 +2129,129 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2244,7 +2389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>

</xml_diff>

<commit_message>
All framed for first test
Investmentblock attribute should be ok. To test with the first case
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>Installed capacity</t>
+  </si>
+  <si>
+    <t>[Nass]</t>
   </si>
 </sst>
 </file>
@@ -2132,7 +2135,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+      <selection activeCell="E2" sqref="E2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2141,7 +2144,7 @@
     <col min="2" max="2" width="22.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2178,8 +2181,8 @@
       <c r="D2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>14</v>
@@ -2198,8 +2201,8 @@
       <c r="D3" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
+      <c r="E3" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>14</v>
@@ -2218,8 +2221,8 @@
       <c r="D4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
+      <c r="E4" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>14</v>
@@ -2238,8 +2241,8 @@
       <c r="D5" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
+      <c r="E5" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
First version capacity expansion uc
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="141">
   <si>
     <t>Name</t>
   </si>
@@ -418,6 +418,42 @@
   </si>
   <si>
     <t>Efficiency</t>
+  </si>
+  <si>
+    <t>BatteryInvestmentCost</t>
+  </si>
+  <si>
+    <t>ConverterInvestmentCost</t>
+  </si>
+  <si>
+    <t>BatteryMaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>ConverterMaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>Battery investment cost</t>
+  </si>
+  <si>
+    <t>Converter investment cost</t>
+  </si>
+  <si>
+    <t>Battery max capacity design</t>
+  </si>
+  <si>
+    <t>Converter max capacity design</t>
+  </si>
+  <si>
+    <t>InvestmentCost</t>
+  </si>
+  <si>
+    <t>MaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>Investment cost</t>
+  </si>
+  <si>
+    <t>Max size</t>
   </si>
 </sst>
 </file>
@@ -741,19 +777,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -893,6 +929,46 @@
         <v>109</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1290,19 +1366,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1629,6 +1705,86 @@
         <v>109</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sector coupled - direct transformation
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -1,27 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\sms\transformation_pypsa_smspp\pypsa2smspp\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="IntermittentUnitBlock"/>
-    <sheet r:id="rId2" sheetId="2" name="ThermalUnitBlock"/>
-    <sheet r:id="rId3" sheetId="3" name="BatteryUnitBlock"/>
-    <sheet r:id="rId4" sheetId="4" name="HydroUnitBlock"/>
-    <sheet r:id="rId5" sheetId="5" name="InvestmentBlock"/>
-    <sheet r:id="rId6" sheetId="6" name="SlackUnitBlock"/>
-    <sheet r:id="rId7" sheetId="7" name="Lines"/>
-    <sheet r:id="rId8" sheetId="8" name="Links"/>
+    <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
+    <sheet name="ThermalUnitBlock" sheetId="2" r:id="rId2"/>
+    <sheet name="BatteryUnitBlock" sheetId="3" r:id="rId3"/>
+    <sheet name="HydroUnitBlock" sheetId="4" r:id="rId4"/>
+    <sheet name="InvestmentBlock" sheetId="5" r:id="rId5"/>
+    <sheet name="SlackUnitBlock" sheetId="6" r:id="rId6"/>
+    <sheet name="Lines" sheetId="7" r:id="rId7"/>
+    <sheet name="Links" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="146">
   <si>
     <t>Name</t>
   </si>
@@ -450,13 +455,21 @@
   </si>
   <si>
     <t>Max size</t>
+  </si>
+  <si>
+    <t>ID of the hyperarch - sector coupled only</t>
+  </si>
+  <si>
+    <t>[NB]</t>
+  </si>
+  <si>
+    <t>HyperArcID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,34 +513,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -538,10 +550,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -579,71 +591,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -671,7 +683,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -694,11 +706,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -707,13 +719,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -723,7 +735,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -732,7 +744,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -741,7 +753,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -749,10 +761,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -825,17 +837,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>137</v>
       </c>
@@ -875,7 +887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
@@ -895,7 +907,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -915,7 +927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -935,7 +947,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -955,7 +967,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -975,7 +987,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>139</v>
       </c>
@@ -995,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>141</v>
       </c>
@@ -1029,18 +1041,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="2" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
@@ -1084,7 +1096,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>122</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>68</v>
       </c>
@@ -1147,7 +1159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>70</v>
       </c>
@@ -1168,7 +1180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1189,7 +1201,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -1210,7 +1222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1231,7 +1243,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -1252,7 +1264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>125</v>
       </c>
@@ -1273,7 +1285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>126</v>
       </c>
@@ -1294,7 +1306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
@@ -1315,7 +1327,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>129</v>
       </c>
@@ -1336,7 +1348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>131</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>104</v>
       </c>
@@ -1378,7 +1390,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>133</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>135</v>
       </c>
@@ -1432,20 +1444,20 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="25.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="30.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +1478,7 @@
       </c>
       <c r="G1" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -1487,7 +1499,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
@@ -1508,7 +1520,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1529,7 +1541,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>54</v>
       </c>
@@ -1550,7 +1562,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>68</v>
       </c>
@@ -1571,7 +1583,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
@@ -1592,7 +1604,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>90</v>
       </c>
@@ -1613,7 +1625,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>92</v>
       </c>
@@ -1634,7 +1646,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>94</v>
       </c>
@@ -1655,7 +1667,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
@@ -1676,7 +1688,7 @@
       </c>
       <c r="G11" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>98</v>
       </c>
@@ -1697,7 +1709,7 @@
       </c>
       <c r="G12" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>100</v>
       </c>
@@ -1718,7 +1730,7 @@
       </c>
       <c r="G13" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
@@ -1739,7 +1751,7 @@
       </c>
       <c r="G14" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>104</v>
       </c>
@@ -1762,7 +1774,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>107</v>
       </c>
@@ -1785,7 +1797,7 @@
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1806,7 +1818,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
@@ -1827,7 +1839,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>112</v>
       </c>
@@ -1848,7 +1860,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>114</v>
       </c>
@@ -1869,7 +1881,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>116</v>
       </c>
@@ -1904,17 +1916,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="16.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="33.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="7.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="15.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1946,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1954,7 +1966,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -1974,7 +1986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1994,7 +2006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -2034,7 +2046,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
@@ -2054,7 +2066,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>48</v>
       </c>
@@ -2094,7 +2106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -2134,7 +2146,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -2154,7 +2166,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -2174,7 +2186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2194,7 +2206,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -2214,7 +2226,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -2234,7 +2246,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>65</v>
       </c>
@@ -2254,7 +2266,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2274,7 +2286,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>72</v>
       </c>
@@ -2314,7 +2326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>74</v>
       </c>
@@ -2334,7 +2346,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>76</v>
       </c>
@@ -2354,7 +2366,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>78</v>
       </c>
@@ -2374,7 +2386,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>80</v>
       </c>
@@ -2408,17 +2420,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="22.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="4.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2438,7 +2450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2458,7 +2470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -2478,7 +2490,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -2498,7 +2510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -2532,17 +2544,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="4.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2562,7 +2573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -2582,7 +2593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -2612,21 +2623,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2646,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2666,7 +2677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2686,7 +2697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2706,7 +2717,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2726,7 +2737,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2746,7 +2757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2764,6 +2775,26 @@
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2776,21 +2807,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="6" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2810,7 +2838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2830,7 +2858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -2850,7 +2878,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -2870,7 +2898,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -2890,7 +2918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -2910,7 +2938,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2928,6 +2956,26 @@
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Direct transf multi-link up to PySMSpp problem
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="147">
   <si>
     <t>Name</t>
   </si>
@@ -464,6 +464,9 @@
   </si>
   <si>
     <t>HyperArcID</t>
+  </si>
+  <si>
+    <t>[Li] | [NB]</t>
   </si>
 </sst>
 </file>
@@ -2626,7 +2629,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2810,7 +2813,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2852,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -2872,7 +2875,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -2952,7 +2955,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added UCBlock expansion parameters
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="153">
   <si>
     <t>Name</t>
   </si>
@@ -467,6 +467,24 @@
   </si>
   <si>
     <t>[Li] | [NB]</t>
+  </si>
+  <si>
+    <t>MinCapacityDesign</t>
+  </si>
+  <si>
+    <t>Min size</t>
+  </si>
+  <si>
+    <t>BatteryMinCapacityDesign</t>
+  </si>
+  <si>
+    <t>ConverterMinCapacityDesign</t>
+  </si>
+  <si>
+    <t>Battery min capacity design</t>
+  </si>
+  <si>
+    <t>Converter min capacity design</t>
   </si>
 </sst>
 </file>
@@ -836,9 +854,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1027,6 +1047,26 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1445,9 +1485,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1904,6 +1946,46 @@
         <v>33</v>
       </c>
       <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2628,7 +2710,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add DesignNetworkBlock - Transformation passed
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="155">
   <si>
     <t>Name</t>
   </si>
@@ -100,391 +100,397 @@
     <t>Cost</t>
   </si>
   <si>
+    <t>LowerBound</t>
+  </si>
+  <si>
+    <t>Minimum acceptable size</t>
+  </si>
+  <si>
+    <t>UpperBound</t>
+  </si>
+  <si>
+    <t>Maximum acceptable size</t>
+  </si>
+  <si>
+    <t>InstalledQuantity</t>
+  </si>
+  <si>
+    <t>Installed capacity</t>
+  </si>
+  <si>
+    <t>NumberReservoirs</t>
+  </si>
+  <si>
+    <t>Number of reservoirs</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>NumberArcs</t>
+  </si>
+  <si>
+    <t>Number of arcs</t>
+  </si>
+  <si>
+    <t>StartArc</t>
+  </si>
+  <si>
+    <t>Starting point of arc</t>
+  </si>
+  <si>
+    <t>[NA]</t>
+  </si>
+  <si>
+    <t>EndArc</t>
+  </si>
+  <si>
+    <t>Ending point of arc</t>
+  </si>
+  <si>
+    <t>MaxVolumetric</t>
+  </si>
+  <si>
+    <t>Maximum volume of reservoir</t>
+  </si>
+  <si>
+    <t>[1][NR] | [T][NR]</t>
+  </si>
+  <si>
+    <t>MinVolumetric</t>
+  </si>
+  <si>
+    <t>Minimum volume of reservoir</t>
+  </si>
+  <si>
+    <t>Inflows</t>
+  </si>
+  <si>
+    <t>[NR][T]</t>
+  </si>
+  <si>
+    <t>MaxFlow</t>
+  </si>
+  <si>
+    <t>Maximum volumetric flow rate</t>
+  </si>
+  <si>
+    <t>[NA] | [T][NA]</t>
+  </si>
+  <si>
+    <t>MinFlow</t>
+  </si>
+  <si>
+    <t>Minimum volumetric flow rate</t>
+  </si>
+  <si>
+    <t>Maximum power output</t>
+  </si>
+  <si>
+    <t>MinPower</t>
+  </si>
+  <si>
+    <t>Minimum power output</t>
+  </si>
+  <si>
+    <t>PrimaryRho</t>
+  </si>
+  <si>
+    <t>Fraction of primary reserve</t>
+  </si>
+  <si>
+    <t>SecondaryRho</t>
+  </si>
+  <si>
+    <t>Fraction of secondary reserve</t>
+  </si>
+  <si>
+    <t>NumberPieces</t>
+  </si>
+  <si>
+    <t>Number of pieces</t>
+  </si>
+  <si>
+    <t>ConstantTerm</t>
+  </si>
+  <si>
+    <t>Constant multiplier of FTAP function</t>
+  </si>
+  <si>
+    <t>[NP]</t>
+  </si>
+  <si>
+    <t>LinearTerm</t>
+  </si>
+  <si>
+    <t>Linear multiplier of FTAP function</t>
+  </si>
+  <si>
+    <t>[NP] | [T][NP]</t>
+  </si>
+  <si>
+    <t>DeltaRampUp</t>
+  </si>
+  <si>
+    <t>Ramp-up limit</t>
+  </si>
+  <si>
+    <t>DeltaRampDown</t>
+  </si>
+  <si>
+    <t>Ramp-down limit</t>
+  </si>
+  <si>
+    <t>DownhillFlow</t>
+  </si>
+  <si>
+    <t>Downhill flow rate</t>
+  </si>
+  <si>
+    <t>UphillFlow</t>
+  </si>
+  <si>
+    <t>Uphill flow rate</t>
+  </si>
+  <si>
+    <t>InertiaPower</t>
+  </si>
+  <si>
+    <t>Inertia power</t>
+  </si>
+  <si>
+    <t>InitialFlowRate</t>
+  </si>
+  <si>
+    <t>Initial flow rate</t>
+  </si>
+  <si>
+    <t>InitialVolumetric</t>
+  </si>
+  <si>
+    <t>Initial volumetric</t>
+  </si>
+  <si>
+    <t>[NR]</t>
+  </si>
+  <si>
+    <t>Kappa</t>
+  </si>
+  <si>
+    <t>Variable to multiply min/max power</t>
+  </si>
+  <si>
+    <t>ConverterMaxPower</t>
+  </si>
+  <si>
+    <t>Maximum power output converter</t>
+  </si>
+  <si>
+    <t>Maximum power output battery</t>
+  </si>
+  <si>
+    <t>Minimum power output battery</t>
+  </si>
+  <si>
+    <t>Rump-down limit</t>
+  </si>
+  <si>
+    <t>ExtractingBatteryRho</t>
+  </si>
+  <si>
+    <t>Discharge efficiency</t>
+  </si>
+  <si>
+    <t>StoringBatteryRho</t>
+  </si>
+  <si>
+    <t>Charge efficiency</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>[T][1]</t>
+  </si>
+  <si>
+    <t>MinStorage</t>
+  </si>
+  <si>
+    <t>Minimum storage level</t>
+  </si>
+  <si>
+    <t>MaxStorage</t>
+  </si>
+  <si>
+    <t>Maximum storage level</t>
+  </si>
+  <si>
+    <t>MaxPrimaryPower</t>
+  </si>
+  <si>
+    <t>Maximum primary reserve power</t>
+  </si>
+  <si>
+    <t>MaxSecondaryPower</t>
+  </si>
+  <si>
+    <t>Maximum secondary reserve power</t>
+  </si>
+  <si>
+    <t>InitialPower</t>
+  </si>
+  <si>
+    <t>Initial power</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>InitialStorage</t>
+  </si>
+  <si>
+    <t>Initial storage</t>
+  </si>
+  <si>
+    <t>Cost function</t>
+  </si>
+  <si>
+    <t>BatteryInvestmentCost</t>
+  </si>
+  <si>
+    <t>Battery investment cost</t>
+  </si>
+  <si>
+    <t>ConverterInvestmentCost</t>
+  </si>
+  <si>
+    <t>Converter investment cost</t>
+  </si>
+  <si>
+    <t>BatteryMaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>Battery max capacity design</t>
+  </si>
+  <si>
+    <t>ConverterMaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>Converter max capacity design</t>
+  </si>
+  <si>
+    <t>Set until</t>
+  </si>
+  <si>
+    <t>InitUpDownTime</t>
+  </si>
+  <si>
+    <t>MinUpTime</t>
+  </si>
+  <si>
+    <t>MaxUpTime</t>
+  </si>
+  <si>
+    <t>MinDownTime</t>
+  </si>
+  <si>
+    <t>Minimum power</t>
+  </si>
+  <si>
+    <t>Maximum power</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>QuadTerm</t>
+  </si>
+  <si>
+    <t>Quadratic term PCF</t>
+  </si>
+  <si>
+    <t>Linear term PCF</t>
+  </si>
+  <si>
+    <t>ConstTerm</t>
+  </si>
+  <si>
+    <t>Constant term PCF</t>
+  </si>
+  <si>
+    <t>StartUpCost</t>
+  </si>
+  <si>
+    <t>Start-up cost</t>
+  </si>
+  <si>
+    <t>FixedConsumption</t>
+  </si>
+  <si>
+    <t>Fixed consumption</t>
+  </si>
+  <si>
+    <t>InertiaCommitment</t>
+  </si>
+  <si>
+    <t>Intertia commitment</t>
+  </si>
+  <si>
+    <t>Gamma</t>
+  </si>
+  <si>
+    <t>Variable for uncertainty in output</t>
+  </si>
+  <si>
+    <t>InvestmentCost</t>
+  </si>
+  <si>
+    <t>Investment cost</t>
+  </si>
+  <si>
+    <t>MaxCapacityDesign</t>
+  </si>
+  <si>
+    <t>Max size</t>
+  </si>
+  <si>
+    <t>ID of the hyperarch - sector coupled only</t>
+  </si>
+  <si>
+    <t>[NB]</t>
+  </si>
+  <si>
+    <t>HyperArcID</t>
+  </si>
+  <si>
+    <t>[Li] | [NB]</t>
+  </si>
+  <si>
+    <t>MinCapacityDesign</t>
+  </si>
+  <si>
+    <t>Min size</t>
+  </si>
+  <si>
+    <t>BatteryMinCapacityDesign</t>
+  </si>
+  <si>
+    <t>ConverterMinCapacityDesign</t>
+  </si>
+  <si>
+    <t>Battery min capacity design</t>
+  </si>
+  <si>
+    <t>Converter min capacity design</t>
+  </si>
+  <si>
     <t>[Nass]</t>
   </si>
   <si>
-    <t>LowerBound</t>
-  </si>
-  <si>
-    <t>Minimum acceptable size</t>
-  </si>
-  <si>
-    <t>UpperBound</t>
-  </si>
-  <si>
-    <t>Maximum acceptable size</t>
-  </si>
-  <si>
-    <t>InstalledQuantity</t>
-  </si>
-  <si>
-    <t>Installed capacity</t>
-  </si>
-  <si>
-    <t>NumberReservoirs</t>
-  </si>
-  <si>
-    <t>Number of reservoirs</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>NumberArcs</t>
-  </si>
-  <si>
-    <t>Number of arcs</t>
-  </si>
-  <si>
-    <t>StartArc</t>
-  </si>
-  <si>
-    <t>Starting point of arc</t>
-  </si>
-  <si>
-    <t>[NA]</t>
-  </si>
-  <si>
-    <t>EndArc</t>
-  </si>
-  <si>
-    <t>Ending point of arc</t>
-  </si>
-  <si>
-    <t>MaxVolumetric</t>
-  </si>
-  <si>
-    <t>Maximum volume of reservoir</t>
-  </si>
-  <si>
-    <t>[1][NR] | [T][NR]</t>
-  </si>
-  <si>
-    <t>MinVolumetric</t>
-  </si>
-  <si>
-    <t>Minimum volume of reservoir</t>
-  </si>
-  <si>
-    <t>Inflows</t>
-  </si>
-  <si>
-    <t>[NR][T]</t>
-  </si>
-  <si>
-    <t>MaxFlow</t>
-  </si>
-  <si>
-    <t>Maximum volumetric flow rate</t>
-  </si>
-  <si>
-    <t>[NA] | [T][NA]</t>
-  </si>
-  <si>
-    <t>MinFlow</t>
-  </si>
-  <si>
-    <t>Minimum volumetric flow rate</t>
-  </si>
-  <si>
-    <t>Maximum power output</t>
-  </si>
-  <si>
-    <t>MinPower</t>
-  </si>
-  <si>
-    <t>Minimum power output</t>
-  </si>
-  <si>
-    <t>PrimaryRho</t>
-  </si>
-  <si>
-    <t>Fraction of primary reserve</t>
-  </si>
-  <si>
-    <t>SecondaryRho</t>
-  </si>
-  <si>
-    <t>Fraction of secondary reserve</t>
-  </si>
-  <si>
-    <t>NumberPieces</t>
-  </si>
-  <si>
-    <t>Number of pieces</t>
-  </si>
-  <si>
-    <t>ConstantTerm</t>
-  </si>
-  <si>
-    <t>Constant multiplier of FTAP function</t>
-  </si>
-  <si>
-    <t>[NP]</t>
-  </si>
-  <si>
-    <t>LinearTerm</t>
-  </si>
-  <si>
-    <t>Linear multiplier of FTAP function</t>
-  </si>
-  <si>
-    <t>[NP] | [T][NP]</t>
-  </si>
-  <si>
-    <t>DeltaRampUp</t>
-  </si>
-  <si>
-    <t>Ramp-up limit</t>
-  </si>
-  <si>
-    <t>DeltaRampDown</t>
-  </si>
-  <si>
-    <t>Ramp-down limit</t>
-  </si>
-  <si>
-    <t>DownhillFlow</t>
-  </si>
-  <si>
-    <t>Downhill flow rate</t>
-  </si>
-  <si>
-    <t>UphillFlow</t>
-  </si>
-  <si>
-    <t>Uphill flow rate</t>
-  </si>
-  <si>
-    <t>InertiaPower</t>
-  </si>
-  <si>
-    <t>Inertia power</t>
-  </si>
-  <si>
-    <t>InitialFlowRate</t>
-  </si>
-  <si>
-    <t>Initial flow rate</t>
-  </si>
-  <si>
-    <t>InitialVolumetric</t>
-  </si>
-  <si>
-    <t>Initial volumetric</t>
-  </si>
-  <si>
-    <t>[NR]</t>
-  </si>
-  <si>
-    <t>Kappa</t>
-  </si>
-  <si>
-    <t>Variable to multiply min/max power</t>
-  </si>
-  <si>
-    <t>ConverterMaxPower</t>
-  </si>
-  <si>
-    <t>Maximum power output converter</t>
-  </si>
-  <si>
-    <t>Maximum power output battery</t>
-  </si>
-  <si>
-    <t>Minimum power output battery</t>
-  </si>
-  <si>
-    <t>Rump-down limit</t>
-  </si>
-  <si>
-    <t>ExtractingBatteryRho</t>
-  </si>
-  <si>
-    <t>Discharge efficiency</t>
-  </si>
-  <si>
-    <t>StoringBatteryRho</t>
-  </si>
-  <si>
-    <t>Charge efficiency</t>
-  </si>
-  <si>
-    <t>Demand</t>
-  </si>
-  <si>
-    <t>[T][1]</t>
-  </si>
-  <si>
-    <t>MinStorage</t>
-  </si>
-  <si>
-    <t>Minimum storage level</t>
-  </si>
-  <si>
-    <t>MaxStorage</t>
-  </si>
-  <si>
-    <t>Maximum storage level</t>
-  </si>
-  <si>
-    <t>MaxPrimaryPower</t>
-  </si>
-  <si>
-    <t>Maximum primary reserve power</t>
-  </si>
-  <si>
-    <t>MaxSecondaryPower</t>
-  </si>
-  <si>
-    <t>Maximum secondary reserve power</t>
-  </si>
-  <si>
-    <t>InitialPower</t>
-  </si>
-  <si>
-    <t>Initial power</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>InitialStorage</t>
-  </si>
-  <si>
-    <t>Initial storage</t>
-  </si>
-  <si>
-    <t>Cost function</t>
-  </si>
-  <si>
-    <t>BatteryInvestmentCost</t>
-  </si>
-  <si>
-    <t>Battery investment cost</t>
-  </si>
-  <si>
-    <t>ConverterInvestmentCost</t>
-  </si>
-  <si>
-    <t>Converter investment cost</t>
-  </si>
-  <si>
-    <t>BatteryMaxCapacityDesign</t>
-  </si>
-  <si>
-    <t>Battery max capacity design</t>
-  </si>
-  <si>
-    <t>ConverterMaxCapacityDesign</t>
-  </si>
-  <si>
-    <t>Converter max capacity design</t>
-  </si>
-  <si>
-    <t>Set until</t>
-  </si>
-  <si>
-    <t>InitUpDownTime</t>
-  </si>
-  <si>
-    <t>MinUpTime</t>
-  </si>
-  <si>
-    <t>MaxUpTime</t>
-  </si>
-  <si>
-    <t>MinDownTime</t>
-  </si>
-  <si>
-    <t>Minimum power</t>
-  </si>
-  <si>
-    <t>Maximum power</t>
-  </si>
-  <si>
-    <t>Availability</t>
-  </si>
-  <si>
-    <t>QuadTerm</t>
-  </si>
-  <si>
-    <t>Quadratic term PCF</t>
-  </si>
-  <si>
-    <t>Linear term PCF</t>
-  </si>
-  <si>
-    <t>ConstTerm</t>
-  </si>
-  <si>
-    <t>Constant term PCF</t>
-  </si>
-  <si>
-    <t>StartUpCost</t>
-  </si>
-  <si>
-    <t>Start-up cost</t>
-  </si>
-  <si>
-    <t>FixedConsumption</t>
-  </si>
-  <si>
-    <t>Fixed consumption</t>
-  </si>
-  <si>
-    <t>InertiaCommitment</t>
-  </si>
-  <si>
-    <t>Intertia commitment</t>
-  </si>
-  <si>
-    <t>Gamma</t>
-  </si>
-  <si>
-    <t>Variable for uncertainty in output</t>
-  </si>
-  <si>
-    <t>InvestmentCost</t>
-  </si>
-  <si>
-    <t>Investment cost</t>
-  </si>
-  <si>
-    <t>MaxCapacityDesign</t>
-  </si>
-  <si>
-    <t>Max size</t>
-  </si>
-  <si>
-    <t>ID of the hyperarch - sector coupled only</t>
-  </si>
-  <si>
-    <t>[NB]</t>
-  </si>
-  <si>
-    <t>HyperArcID</t>
-  </si>
-  <si>
-    <t>[Li] | [NB]</t>
-  </si>
-  <si>
-    <t>MinCapacityDesign</t>
-  </si>
-  <si>
-    <t>Min size</t>
-  </si>
-  <si>
-    <t>BatteryMinCapacityDesign</t>
-  </si>
-  <si>
-    <t>ConverterMinCapacityDesign</t>
-  </si>
-  <si>
-    <t>Battery min capacity design</t>
-  </si>
-  <si>
-    <t>Converter min capacity design</t>
+    <t>Capital cost if only lines</t>
+  </si>
+  <si>
+    <t>[NDL]</t>
   </si>
 </sst>
 </file>
@@ -892,10 +898,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -907,15 +913,15 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -927,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -935,7 +941,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -952,10 +958,10 @@
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -972,10 +978,10 @@
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -987,7 +993,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -995,7 +1001,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -1007,15 +1013,15 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1027,15 +1033,15 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -1047,15 +1053,15 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -1067,7 +1073,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1112,7 +1118,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1120,10 +1126,10 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1136,15 +1142,15 @@
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1157,15 +1163,15 @@
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1178,15 +1184,15 @@
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1199,15 +1205,15 @@
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -1220,15 +1226,15 @@
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -1249,7 +1255,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1267,10 +1273,10 @@
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -1283,15 +1289,15 @@
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
@@ -1304,15 +1310,15 @@
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -1325,15 +1331,15 @@
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1346,15 +1352,15 @@
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1367,15 +1373,15 @@
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -1388,15 +1394,15 @@
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1409,15 +1415,15 @@
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -1430,15 +1436,15 @@
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1451,15 +1457,15 @@
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1472,7 +1478,7 @@
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1493,7 @@
   </sheetPr>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -1525,10 +1531,10 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1540,16 +1546,16 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -1570,7 +1576,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -1588,10 +1594,10 @@
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1609,10 +1615,10 @@
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -1624,16 +1630,16 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
@@ -1645,16 +1651,16 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
@@ -1666,16 +1672,16 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
@@ -1687,37 +1693,37 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -1735,10 +1741,10 @@
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1756,10 +1762,10 @@
     </row>
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1771,16 +1777,16 @@
         <v>20</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
@@ -1792,16 +1798,16 @@
         <v>20</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1813,18 +1819,18 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -1836,10 +1842,10 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1847,7 +1853,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1859,16 +1865,16 @@
         <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
@@ -1880,16 +1886,16 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
@@ -1901,16 +1907,16 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -1922,16 +1928,16 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
@@ -1943,16 +1949,16 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
@@ -1964,15 +1970,15 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
@@ -1984,7 +1990,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2033,10 +2039,10 @@
     </row>
     <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -2048,15 +2054,15 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -2073,10 +2079,10 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -2085,7 +2091,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -2093,10 +2099,10 @@
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -2105,7 +2111,7 @@
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>10</v>
@@ -2113,31 +2119,31 @@
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2145,59 +2151,59 @@
         <v>13</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
@@ -2205,10 +2211,10 @@
         <v>13</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2216,7 +2222,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
@@ -2225,19 +2231,19 @@
         <v>13</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -2245,19 +2251,19 @@
         <v>13</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2265,19 +2271,19 @@
         <v>13</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2285,18 +2291,18 @@
         <v>13</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -2305,7 +2311,7 @@
         <v>8</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>10</v>
@@ -2313,19 +2319,19 @@
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -2333,19 +2339,19 @@
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>10</v>
@@ -2353,11 +2359,11 @@
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
@@ -2365,19 +2371,19 @@
         <v>13</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
@@ -2385,18 +2391,18 @@
         <v>13</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>7</v>
@@ -2405,18 +2411,18 @@
         <v>8</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>7</v>
@@ -2425,19 +2431,19 @@
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
@@ -2445,19 +2451,19 @@
         <v>13</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
@@ -2465,27 +2471,27 @@
         <v>13</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>10</v>
@@ -2501,17 +2507,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2549,7 +2557,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -2557,11 +2565,11 @@
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2569,7 +2577,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -2577,11 +2585,11 @@
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
@@ -2589,7 +2597,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
@@ -2597,11 +2605,11 @@
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2609,9 +2617,69 @@
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2864,22 +2932,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -2937,7 +3005,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -2957,7 +3025,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
@@ -3037,7 +3105,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>10</v>
@@ -3045,22 +3113,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction on lines expansion if some expand and others do not
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -490,7 +490,7 @@
     <t>Capital cost if only lines</t>
   </si>
   <si>
-    <t>[NDL]</t>
+    <t>[NDL] | [NDLL] | [NDLLi]</t>
   </si>
 </sst>
 </file>
@@ -2519,7 +2519,7 @@
     <col min="2" max="2" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
NetworkCost included for lines
</commit_message>
<xml_diff>
--- a/pypsa2smspp/data/smspp_parameters.xlsx
+++ b/pypsa2smspp/data/smspp_parameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="IntermittentUnitBlock" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>[NDL] | [NDLL] | [NDLLi]</t>
+  </si>
+  <si>
+    <t>NetworkCost</t>
+  </si>
+  <si>
+    <t>Marginal cost of the line</t>
   </si>
 </sst>
 </file>
@@ -2509,7 +2515,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6:E8"/>
     </sheetView>
   </sheetViews>
@@ -2776,10 +2782,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E7"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2950,6 +2956,26 @@
         <v>32</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2960,10 +2986,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,21 +3139,41 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>